<commit_message>
Reworded some code comments and improved look of excel output file
</commit_message>
<xml_diff>
--- a/eA_template.xlsx
+++ b/eA_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="mc" sheetId="38" r:id="rId1"/>
@@ -304,10 +304,10 @@
     <t>ABC</t>
   </si>
   <si>
-    <t>XYX</t>
-  </si>
-  <si>
     <t>ZZZ</t>
+  </si>
+  <si>
+    <t>XYZ</t>
   </si>
 </sst>
 </file>
@@ -876,11 +876,11 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -920,10 +920,10 @@
         <v>88</v>
       </c>
       <c r="C7" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="28" t="s">
         <v>89</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1078,7 +1078,7 @@
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="B9:D19"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1119,10 +1119,10 @@
         <v>88</v>
       </c>
       <c r="C7" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="28" t="s">
         <v>89</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1320,7 +1320,7 @@
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1361,10 +1361,10 @@
         <v>88</v>
       </c>
       <c r="C7" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="28" t="s">
         <v>89</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1688,7 +1688,7 @@
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1728,10 +1728,10 @@
         <v>88</v>
       </c>
       <c r="C7" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="28" t="s">
         <v>89</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2036,11 +2036,11 @@
   </sheetPr>
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2081,10 +2081,10 @@
         <v>88</v>
       </c>
       <c r="C7" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="28" t="s">
         <v>89</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -3152,6 +3152,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3160,7 +3166,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="----- General Document -----" ma:contentTypeID="0x0101000945343AC7418640832878951C0DA04C0010F4303BE228A84F8F3E9BA01A6019AD" ma:contentTypeVersion="2" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="3a55d3cb885f8b8d3a603081f3ea71b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="04ea406deab3b3fd3b4cd009fdbc55ac">
     <xsd:element name="properties">
@@ -3274,13 +3280,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21B9D63C-2314-4030-99CE-A9B829F845F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E38FFF8D-2BEA-4A16-B864-D8E0AC74490A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -3288,7 +3303,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{180A7F46-5AD0-47B9-A99E-B57403F75C9F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3302,19 +3317,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21B9D63C-2314-4030-99CE-A9B829F845F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>